<commit_message>
Forecast with adjusted beds v0.1
</commit_message>
<xml_diff>
--- a/app/templates/report/forecast.xlsx
+++ b/app/templates/report/forecast.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\Development\projects\ciber\cotown\back\app\templates\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33E2E646-D37A-4C44-842E-E382B73B69B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2536142-A312-43D1-8265-9B98F4776030}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Forecast!$A$4:$B$4</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterate="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="48">
   <si>
     <t>Resource</t>
   </si>
@@ -200,6 +200,10 @@
   <si>
     <t>Booking
 fee</t>
+  </si>
+  <si>
+    <t>Adj.
+Beds</t>
   </si>
 </sst>
 </file>
@@ -274,7 +278,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -335,6 +339,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="20">
     <border>
@@ -576,7 +592,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -732,6 +748,10 @@
     </xf>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="2" fillId="4" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hipervínculo 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
@@ -1132,7 +1152,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AP5"/>
+  <dimension ref="A1:AQ5"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
@@ -1146,22 +1166,22 @@
     <col min="1" max="1" width="9.85546875" style="25" customWidth="1"/>
     <col min="2" max="2" width="14.140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="10.5703125" style="1" customWidth="1"/>
-    <col min="4" max="7" width="6.5703125" style="1" customWidth="1"/>
-    <col min="8" max="10" width="8.140625" style="1" customWidth="1"/>
-    <col min="11" max="14" width="9.140625" style="1" customWidth="1"/>
-    <col min="15" max="22" width="8.85546875" style="1" customWidth="1"/>
-    <col min="23" max="26" width="11.42578125" style="1" customWidth="1"/>
-    <col min="27" max="30" width="12.7109375" style="1" customWidth="1"/>
-    <col min="31" max="33" width="11.42578125" style="1" customWidth="1"/>
-    <col min="34" max="35" width="8.85546875" style="1" customWidth="1"/>
-    <col min="36" max="37" width="8.5703125" style="1" customWidth="1"/>
-    <col min="38" max="39" width="12.7109375" style="1" customWidth="1"/>
-    <col min="40" max="41" width="8.5703125" style="1" customWidth="1"/>
-    <col min="42" max="42" width="12.7109375" style="1" customWidth="1"/>
-    <col min="43" max="16384" width="14.42578125" style="1"/>
+    <col min="4" max="8" width="6.5703125" style="1" customWidth="1"/>
+    <col min="9" max="11" width="8.140625" style="1" customWidth="1"/>
+    <col min="12" max="15" width="9.140625" style="1" customWidth="1"/>
+    <col min="16" max="23" width="8.85546875" style="1" customWidth="1"/>
+    <col min="24" max="27" width="11.42578125" style="1" customWidth="1"/>
+    <col min="28" max="31" width="12.7109375" style="1" customWidth="1"/>
+    <col min="32" max="34" width="11.42578125" style="1" customWidth="1"/>
+    <col min="35" max="36" width="8.85546875" style="1" customWidth="1"/>
+    <col min="37" max="38" width="8.5703125" style="1" customWidth="1"/>
+    <col min="39" max="40" width="12.7109375" style="1" customWidth="1"/>
+    <col min="41" max="42" width="8.5703125" style="1" customWidth="1"/>
+    <col min="43" max="43" width="12.7109375" style="1" customWidth="1"/>
+    <col min="44" max="16384" width="14.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:43" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
         <v>17</v>
       </c>
@@ -1175,11 +1195,11 @@
       </c>
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="3" t="s">
+      <c r="G1" s="5"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="5"/>
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
@@ -1193,32 +1213,33 @@
       <c r="T1" s="5"/>
       <c r="U1" s="5"/>
       <c r="V1" s="5"/>
-      <c r="W1" s="21"/>
+      <c r="W1" s="5"/>
       <c r="X1" s="21"/>
       <c r="Y1" s="21"/>
-      <c r="Z1" s="6"/>
-      <c r="AA1" s="5"/>
+      <c r="Z1" s="21"/>
+      <c r="AA1" s="6"/>
       <c r="AB1" s="5"/>
       <c r="AC1" s="5"/>
       <c r="AD1" s="5"/>
-      <c r="AE1" s="6"/>
-      <c r="AF1" s="5"/>
+      <c r="AE1" s="5"/>
+      <c r="AF1" s="6"/>
       <c r="AG1" s="5"/>
-      <c r="AH1" s="3" t="s">
+      <c r="AH1" s="5"/>
+      <c r="AI1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="AI1" s="5"/>
       <c r="AJ1" s="5"/>
       <c r="AK1" s="5"/>
       <c r="AL1" s="5"/>
-      <c r="AM1" s="6"/>
-      <c r="AN1" s="3" t="s">
+      <c r="AM1" s="5"/>
+      <c r="AN1" s="6"/>
+      <c r="AO1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="AO1" s="5"/>
-      <c r="AP1" s="6"/>
+      <c r="AP1" s="5"/>
+      <c r="AQ1" s="6"/>
     </row>
-    <row r="2" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
         <v>30</v>
       </c>
@@ -1234,138 +1255,140 @@
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="8"/>
+      <c r="I2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="8"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="7" t="s">
+      <c r="J2" s="8"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="L2" s="8"/>
       <c r="M2" s="8"/>
-      <c r="N2" s="9"/>
-      <c r="O2" s="7"/>
-      <c r="P2" s="8"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="9"/>
+      <c r="P2" s="7"/>
       <c r="Q2" s="8"/>
-      <c r="R2" s="9"/>
-      <c r="S2" s="7" t="s">
+      <c r="R2" s="8"/>
+      <c r="S2" s="9"/>
+      <c r="T2" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="T2" s="8"/>
       <c r="U2" s="8"/>
-      <c r="V2" s="9"/>
-      <c r="W2" s="22" t="s">
+      <c r="V2" s="8"/>
+      <c r="W2" s="9"/>
+      <c r="X2" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="X2" s="22"/>
       <c r="Y2" s="22"/>
-      <c r="Z2" s="9"/>
-      <c r="AA2" s="8"/>
+      <c r="Z2" s="22"/>
+      <c r="AA2" s="9"/>
       <c r="AB2" s="8"/>
       <c r="AC2" s="8"/>
       <c r="AD2" s="8"/>
-      <c r="AE2" s="80" t="s">
+      <c r="AE2" s="8"/>
+      <c r="AF2" s="80" t="s">
         <v>40</v>
       </c>
-      <c r="AF2" s="8"/>
       <c r="AG2" s="8"/>
-      <c r="AH2" s="7" t="s">
+      <c r="AH2" s="8"/>
+      <c r="AI2" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="AI2" s="8"/>
-      <c r="AJ2" s="8" t="s">
+      <c r="AJ2" s="8"/>
+      <c r="AK2" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="AK2" s="8"/>
       <c r="AL2" s="8"/>
-      <c r="AM2" s="9"/>
-      <c r="AN2" s="8" t="s">
+      <c r="AM2" s="8"/>
+      <c r="AN2" s="9"/>
+      <c r="AO2" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="AO2" s="8"/>
-      <c r="AP2" s="9"/>
+      <c r="AP2" s="8"/>
+      <c r="AQ2" s="9"/>
     </row>
-    <row r="3" spans="1:42" s="48" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:43" s="48" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="30"/>
       <c r="B3" s="31"/>
       <c r="C3" s="65"/>
       <c r="D3" s="32"/>
       <c r="E3" s="33"/>
       <c r="F3" s="33"/>
-      <c r="G3" s="34"/>
-      <c r="H3" s="35"/>
-      <c r="I3" s="36"/>
-      <c r="J3" s="37"/>
-      <c r="K3" s="38"/>
-      <c r="L3" s="39"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="35"/>
+      <c r="J3" s="36"/>
+      <c r="K3" s="37"/>
+      <c r="L3" s="38"/>
       <c r="M3" s="39"/>
-      <c r="N3" s="40"/>
-      <c r="O3" s="41"/>
-      <c r="P3" s="42"/>
+      <c r="N3" s="39"/>
+      <c r="O3" s="40"/>
+      <c r="P3" s="41"/>
       <c r="Q3" s="42"/>
-      <c r="R3" s="43"/>
-      <c r="S3" s="44">
+      <c r="R3" s="42"/>
+      <c r="S3" s="43"/>
+      <c r="T3" s="44">
         <v>0.28999999999999998</v>
-      </c>
-      <c r="T3" s="45">
-        <v>0.05</v>
       </c>
       <c r="U3" s="45">
         <v>0.05</v>
       </c>
-      <c r="V3" s="46">
+      <c r="V3" s="45">
+        <v>0.05</v>
+      </c>
+      <c r="W3" s="46">
         <v>0.1</v>
       </c>
-      <c r="W3" s="62">
-        <f>SUM(W5:W1048576)</f>
-        <v>0</v>
-      </c>
       <c r="X3" s="62">
-        <f t="shared" ref="X3:AD3" si="0">SUM(X5:X1048576)</f>
+        <f>SUM(X5:X1048576)</f>
         <v>0</v>
       </c>
       <c r="Y3" s="62">
+        <f t="shared" ref="Y3:AA3" si="0">SUM(Y5:Y1048576)</f>
+        <v>0</v>
+      </c>
+      <c r="Z3" s="62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Z3" s="63">
+      <c r="AA3" s="63">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AA3" s="77">
-        <f t="shared" ref="AA3" si="1">SUM(AA5:AA1048576)</f>
-        <v>0</v>
-      </c>
-      <c r="AB3" s="77"/>
+      <c r="AB3" s="77">
+        <f t="shared" ref="AB3" si="1">SUM(AB5:AB1048576)</f>
+        <v>0</v>
+      </c>
       <c r="AC3" s="77"/>
-      <c r="AD3" s="64">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AE3" s="62"/>
+      <c r="AD3" s="77"/>
+      <c r="AE3" s="64">
+        <f>SUM(AE5:AE1048576)</f>
+        <v>0</v>
+      </c>
       <c r="AF3" s="62"/>
       <c r="AG3" s="62"/>
-      <c r="AH3" s="41"/>
-      <c r="AI3" s="43"/>
-      <c r="AJ3" s="47"/>
-      <c r="AK3" s="70"/>
-      <c r="AL3" s="72">
-        <f t="shared" ref="AL3" si="2">SUM(AL5:AL1048576)</f>
-        <v>0</v>
-      </c>
-      <c r="AM3" s="74">
-        <f>SUM(AM5:AM1048576)</f>
-        <v>0</v>
-      </c>
-      <c r="AN3" s="47"/>
-      <c r="AO3" s="70"/>
-      <c r="AP3" s="74">
-        <f>SUM(AP5:AP1048576)</f>
+      <c r="AH3" s="62"/>
+      <c r="AI3" s="41"/>
+      <c r="AJ3" s="43"/>
+      <c r="AK3" s="47"/>
+      <c r="AL3" s="70"/>
+      <c r="AM3" s="72">
+        <f t="shared" ref="AM3" si="2">SUM(AM5:AM1048576)</f>
+        <v>0</v>
+      </c>
+      <c r="AN3" s="74">
+        <f>SUM(AN5:AN1048576)</f>
+        <v>0</v>
+      </c>
+      <c r="AO3" s="47"/>
+      <c r="AP3" s="70"/>
+      <c r="AQ3" s="74">
+        <f>SUM(AQ5:AQ1048576)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:42" s="18" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:43" s="18" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A4" s="66" t="s">
         <v>31</v>
       </c>
@@ -1381,119 +1404,122 @@
       <c r="E4" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="55" t="s">
+      <c r="F4" s="83" t="s">
+        <v>47</v>
+      </c>
+      <c r="G4" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="55" t="s">
+      <c r="H4" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="56" t="s">
+      <c r="I4" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="I4" s="54" t="s">
+      <c r="J4" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="57" t="s">
+      <c r="K4" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="K4" s="53" t="s">
+      <c r="L4" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="L4" s="58" t="s">
+      <c r="M4" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="M4" s="58" t="s">
+      <c r="N4" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="N4" s="59" t="s">
+      <c r="O4" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="O4" s="56" t="s">
+      <c r="P4" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="P4" s="55" t="s">
+      <c r="Q4" s="55" t="s">
         <v>25</v>
       </c>
-      <c r="Q4" s="55" t="s">
+      <c r="R4" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="R4" s="57" t="s">
+      <c r="S4" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="S4" s="56" t="s">
+      <c r="T4" s="56" t="s">
         <v>32</v>
       </c>
-      <c r="T4" s="55" t="s">
+      <c r="U4" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="U4" s="55" t="s">
+      <c r="V4" s="55" t="s">
         <v>34</v>
       </c>
-      <c r="V4" s="59" t="s">
+      <c r="W4" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="W4" s="60" t="s">
+      <c r="X4" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="X4" s="54" t="s">
+      <c r="Y4" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="Y4" s="54" t="s">
+      <c r="Z4" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="Z4" s="54" t="s">
+      <c r="AA4" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="AA4" s="60" t="s">
+      <c r="AB4" s="60" t="s">
         <v>44</v>
       </c>
-      <c r="AB4" s="56" t="s">
+      <c r="AC4" s="56" t="s">
         <v>45</v>
       </c>
-      <c r="AC4" s="56" t="s">
+      <c r="AD4" s="56" t="s">
         <v>46</v>
       </c>
-      <c r="AD4" s="69" t="s">
+      <c r="AE4" s="69" t="s">
         <v>39</v>
       </c>
-      <c r="AE4" s="60" t="s">
+      <c r="AF4" s="60" t="s">
         <v>41</v>
       </c>
-      <c r="AF4" s="54" t="s">
+      <c r="AG4" s="54" t="s">
         <v>42</v>
       </c>
-      <c r="AG4" s="54" t="s">
+      <c r="AH4" s="54" t="s">
         <v>43</v>
       </c>
-      <c r="AH4" s="56" t="s">
+      <c r="AI4" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="AI4" s="57" t="s">
+      <c r="AJ4" s="57" t="s">
         <v>25</v>
       </c>
-      <c r="AJ4" s="60" t="s">
+      <c r="AK4" s="60" t="s">
         <v>28</v>
       </c>
-      <c r="AK4" s="55" t="s">
+      <c r="AL4" s="55" t="s">
         <v>29</v>
       </c>
-      <c r="AL4" s="60" t="s">
+      <c r="AM4" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="AM4" s="69" t="s">
+      <c r="AN4" s="69" t="s">
         <v>44</v>
       </c>
-      <c r="AN4" s="56" t="s">
+      <c r="AO4" s="56" t="s">
         <v>22</v>
       </c>
-      <c r="AO4" s="55" t="s">
+      <c r="AP4" s="55" t="s">
         <v>23</v>
       </c>
-      <c r="AP4" s="69" t="s">
+      <c r="AQ4" s="69" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A5" s="27" t="s">
         <v>36</v>
       </c>
@@ -1501,102 +1527,103 @@
       <c r="C5" s="67"/>
       <c r="D5" s="29"/>
       <c r="E5" s="68"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="2">
-        <f>H5*E5</f>
-        <v>0</v>
-      </c>
-      <c r="J5" s="11">
-        <f>IF(D5&lt;&gt;0,I5/D5,0)</f>
-        <v>0</v>
-      </c>
-      <c r="K5" s="49"/>
-      <c r="L5" s="50"/>
+      <c r="F5" s="84"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="2">
+        <f>I5*E5</f>
+        <v>0</v>
+      </c>
+      <c r="K5" s="11">
+        <f>IF(D5&lt;&gt;0,J5/D5,0)</f>
+        <v>0</v>
+      </c>
+      <c r="L5" s="49"/>
       <c r="M5" s="50"/>
-      <c r="N5" s="51"/>
-      <c r="O5" s="13"/>
-      <c r="P5" s="14"/>
+      <c r="N5" s="50"/>
+      <c r="O5" s="51"/>
+      <c r="P5" s="13"/>
       <c r="Q5" s="14"/>
-      <c r="R5" s="26">
-        <f>1-SUM(O5:Q5)</f>
+      <c r="R5" s="14"/>
+      <c r="S5" s="26">
+        <f>1-SUM(P5:R5)</f>
         <v>1</v>
       </c>
-      <c r="S5" s="15"/>
-      <c r="T5" s="16"/>
+      <c r="T5" s="15"/>
       <c r="U5" s="16"/>
-      <c r="V5" s="17"/>
-      <c r="W5" s="61">
-        <f>(1-SUMPRODUCT($S$3:$V$3,$S5:$V5))*K5*$I5*O5</f>
-        <v>0</v>
-      </c>
+      <c r="V5" s="16"/>
+      <c r="W5" s="17"/>
       <c r="X5" s="61">
-        <f>(1-SUMPRODUCT($S$3:$V$3,$S5:$V5))*L5*$I5*P5</f>
+        <f>(1-SUMPRODUCT($T$3:$W$3,$T5:$W5))*L5*$J5*P5</f>
         <v>0</v>
       </c>
       <c r="Y5" s="61">
-        <f>(1-SUMPRODUCT($S$3:$V$3,$S5:$V5))*M5*$I5*Q5</f>
-        <v>0</v>
-      </c>
-      <c r="Z5" s="76">
-        <f>(1-SUMPRODUCT($S$3:$V$3,$S5:$V5))*N5*$I5*R5</f>
-        <v>0</v>
-      </c>
-      <c r="AA5" s="78">
-        <f>SUM(W5:Z5)</f>
-        <v>0</v>
-      </c>
-      <c r="AB5" s="82"/>
+        <f>(1-SUMPRODUCT($T$3:$W$3,$T5:$W5))*M5*$J5*Q5</f>
+        <v>0</v>
+      </c>
+      <c r="Z5" s="61">
+        <f>(1-SUMPRODUCT($T$3:$W$3,$T5:$W5))*N5*$J5*R5</f>
+        <v>0</v>
+      </c>
+      <c r="AA5" s="76">
+        <f>(1-SUMPRODUCT($T$3:$W$3,$T5:$W5))*O5*$J5*S5</f>
+        <v>0</v>
+      </c>
+      <c r="AB5" s="78">
+        <f>SUM(X5:AA5)</f>
+        <v>0</v>
+      </c>
       <c r="AC5" s="82"/>
-      <c r="AD5" s="79">
-        <f>IF(OR(B5="PFC002",B5="SAR326"),AA5/1.1*C5,AA5*C5)</f>
-        <v>0</v>
-      </c>
-      <c r="AE5" s="61">
-        <f>IF(I5,AA5/I5,0)</f>
+      <c r="AD5" s="82"/>
+      <c r="AE5" s="79">
+        <f>IF(OR(B5="PFC002",B5="SAR326"),AB5/1.1*C5,AB5*C5)</f>
         <v>0</v>
       </c>
       <c r="AF5" s="61">
-        <f>IF(D5,AA5/D5,0)</f>
+        <f>IF(J5,AB5/J5,0)</f>
         <v>0</v>
       </c>
       <c r="AG5" s="61">
-        <f>SUMPRODUCT(K5:N5,O5:R5)</f>
-        <v>0</v>
-      </c>
-      <c r="AH5" s="13"/>
-      <c r="AI5" s="26">
-        <f>1-AH5</f>
+        <f>IF(D5,AB5/D5,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AH5" s="61">
+        <f>SUMPRODUCT(L5:O5,P5:S5)</f>
+        <v>0</v>
+      </c>
+      <c r="AI5" s="13"/>
+      <c r="AJ5" s="26">
+        <f>1-AI5</f>
         <v>1</v>
       </c>
-      <c r="AJ5" s="81">
-        <f>AH5*K5+AI5*L5</f>
-        <v>0</v>
-      </c>
-      <c r="AK5" s="71"/>
-      <c r="AL5" s="73">
-        <f>AJ5*D5</f>
-        <v>0</v>
-      </c>
-      <c r="AM5" s="75">
-        <f t="shared" ref="AM5" si="3">AJ5*D5*AK5</f>
-        <v>0</v>
-      </c>
-      <c r="AN5" s="52"/>
-      <c r="AO5" s="71">
-        <f>AK5</f>
-        <v>0</v>
-      </c>
-      <c r="AP5" s="75">
-        <f>AN5*AO5*G5</f>
+      <c r="AK5" s="81">
+        <f>AI5*L5+AJ5*M5</f>
+        <v>0</v>
+      </c>
+      <c r="AL5" s="71"/>
+      <c r="AM5" s="73">
+        <f>AK5*D5</f>
+        <v>0</v>
+      </c>
+      <c r="AN5" s="75">
+        <f>AK5*D5*AL5</f>
+        <v>0</v>
+      </c>
+      <c r="AO5" s="52"/>
+      <c r="AP5" s="71">
+        <f>AL5</f>
+        <v>0</v>
+      </c>
+      <c r="AQ5" s="75">
+        <f>AO5*AP5*H5</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A4:B4" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="9" type="noConversion"/>
-  <conditionalFormatting sqref="A5:AP99999">
+  <conditionalFormatting sqref="A5:AQ99999">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$B5&lt;&gt;$B4</formula>
     </cfRule>
@@ -1604,7 +1631,7 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <ignoredErrors>
-    <ignoredError sqref="R5" formulaRange="1"/>
+    <ignoredError sqref="S5" formulaRange="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>